<commit_message>
Regression test suite for register page
</commit_message>
<xml_diff>
--- a/manual_tests/Sanity_Suite_0.1.xlsx
+++ b/manual_tests/Sanity_Suite_0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ebfd5dc42167825/Desktop/Testing/Mamta_Mobiles/manual_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{A52E64EC-7A94-4E25-87B6-81A59B369C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{932E3263-E634-4D31-A962-536A50C0698B}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{A52E64EC-7A94-4E25-87B6-81A59B369C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{406F131D-507F-4CE4-9FF9-8F60BDDB195B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,7 +326,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -439,14 +439,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -456,6 +448,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -643,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -746,22 +753,25 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -779,6 +789,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1139,8 +1153,8 @@
   </sheetPr>
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="G8" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1473,40 +1487,40 @@
     </row>
     <row r="10" spans="1:29" ht="27.75" customHeight="1">
       <c r="A10" s="15"/>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="36" t="s">
+      <c r="K10" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="36" t="s">
+      <c r="L10" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="36" t="s">
+      <c r="M10" s="42" t="s">
         <v>19</v>
       </c>
       <c r="N10" s="16"/>
@@ -1528,38 +1542,38 @@
     </row>
     <row r="11" spans="1:29" ht="41.4">
       <c r="A11" s="6"/>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="37" t="s">
+      <c r="I11" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37" t="s">
+      <c r="L11" s="36"/>
+      <c r="M11" s="36" t="s">
         <v>62</v>
       </c>
       <c r="N11" s="18"/>
@@ -1581,38 +1595,38 @@
     </row>
     <row r="12" spans="1:29" ht="41.4">
       <c r="A12" s="6"/>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="37" t="s">
+      <c r="I12" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="K12" s="39" t="s">
+      <c r="K12" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37" t="s">
+      <c r="L12" s="36"/>
+      <c r="M12" s="36" t="s">
         <v>70</v>
       </c>
       <c r="N12" s="18"/>
@@ -1634,38 +1648,38 @@
     </row>
     <row r="13" spans="1:29" ht="41.4">
       <c r="A13" s="6"/>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="37" t="s">
+      <c r="I13" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="J13" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="39" t="s">
+      <c r="K13" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37" t="s">
+      <c r="L13" s="36"/>
+      <c r="M13" s="36" t="s">
         <v>75</v>
       </c>
       <c r="N13" s="18"/>
@@ -1687,38 +1701,38 @@
     </row>
     <row r="14" spans="1:29" ht="41.4">
       <c r="A14" s="6"/>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="37" t="s">
+      <c r="I14" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="39" t="s">
+      <c r="K14" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37" t="s">
+      <c r="L14" s="36"/>
+      <c r="M14" s="36" t="s">
         <v>81</v>
       </c>
       <c r="N14" s="18"/>
@@ -1740,38 +1754,38 @@
     </row>
     <row r="15" spans="1:29" ht="41.4">
       <c r="A15" s="6"/>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="37" t="s">
+      <c r="I15" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="K15" s="39" t="s">
+      <c r="K15" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37" t="s">
+      <c r="L15" s="36"/>
+      <c r="M15" s="36" t="s">
         <v>86</v>
       </c>
       <c r="N15" s="18"/>

</xml_diff>